<commit_message>
reporte con tipos de oficios
</commit_message>
<xml_diff>
--- a/public/reportes/auditoria.xlsx
+++ b/public/reportes/auditoria.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
   <si>
     <t>Año de Auditoría:</t>
   </si>
@@ -44,42 +44,60 @@
     <t>CONTESTACIÓN ÓRGANO FISCALIZADOR</t>
   </si>
   <si>
+    <t>RESPUESTA A CONTESTACIÓN ÓRGANO FISCALIZADOR</t>
+  </si>
+  <si>
     <t>ADMINISTRACIÓN DE RESULTADOS</t>
   </si>
   <si>
     <t>SE SOLICITA INFORMACIÓN PRELIMINAR A LAS DIRECCIONES DE LA SFYTGE:</t>
   </si>
   <si>
+    <t>OFICIO ORDEN</t>
+  </si>
+  <si>
+    <t>FECHA OFICIO</t>
+  </si>
+  <si>
+    <t>OFICIO NOTIFICACIÓN</t>
+  </si>
+  <si>
+    <t>FECHA VENCIMIENTO</t>
+  </si>
+  <si>
+    <t>OFICIO SOLICITUD</t>
+  </si>
+  <si>
+    <t>FECHA SOLICITUD</t>
+  </si>
+  <si>
+    <t>UNIDAD ADMINISTRATIVA</t>
+  </si>
+  <si>
     <t>OFICIO</t>
   </si>
   <si>
-    <t>FECHA VENCIMIENTO</t>
-  </si>
-  <si>
-    <t>TIPO OFICIO</t>
-  </si>
-  <si>
-    <t>UNIDAD ADMINISTRATIVA</t>
-  </si>
-  <si>
-    <t>FECHA OFICIO</t>
-  </si>
-  <si>
     <t>FECHA RECIBIDO</t>
   </si>
   <si>
-    <t>PRÓRROGA</t>
-  </si>
-  <si>
     <t>ÓRGANO</t>
   </si>
   <si>
     <t>FOLIO SIGA</t>
   </si>
   <si>
+    <t>ENTREGA</t>
+  </si>
+  <si>
     <t>FECHA VENCIMENTO</t>
   </si>
   <si>
+    <t>ÓRGANO ORIGEN</t>
+  </si>
+  <si>
+    <t>ÓRGANO DESTINO</t>
+  </si>
+  <si>
     <t>TIPO DE RESULTADO</t>
   </si>
   <si>
@@ -110,78 +128,236 @@
     <t>SOLICITUD</t>
   </si>
   <si>
-    <t>Transferencia de Recursos de los
-Subsidios Federales para Organismos
-Descentralizados Estatales de Educación
-Media Superior y Superior en su Vertiente
-Tecnológica y Politécnica
-U006</t>
-  </si>
-  <si>
-    <t>Dirección General de Auditoría del Gasto Federalizado "A"</t>
+    <t>Cumplimiento de las Disposiciones Establecidas en la Ley de Disciplina Financiera de las Entidades Federativas y
+los Municipios</t>
+  </si>
+  <si>
+    <t>Dirección General de Auditoría del Gasto Federalizado "C"</t>
   </si>
   <si>
     <t>Programa Anual de Auditorías para la Fiscalización Superior (PAAF)</t>
   </si>
   <si>
-    <t>ACTA DE INICIO 1342</t>
-  </si>
-  <si>
-    <t>CTG-DCASC-204-2023</t>
-  </si>
-  <si>
-    <t>2023-03-31</t>
+    <t>2022_1326_AFITAME_001</t>
+  </si>
+  <si>
+    <t>AEGF-5045-2023</t>
+  </si>
+  <si>
+    <t>2023-05-20</t>
+  </si>
+  <si>
+    <t>CTG-DCASC-459-2023</t>
+  </si>
+  <si>
+    <t>2023-05-26</t>
+  </si>
+  <si>
+    <t>prueba de oficio 2</t>
+  </si>
+  <si>
+    <t>prueba de oficio 1</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN DE CONTABILIDAD Y CUENTA PÚBLICA</t>
+  </si>
+  <si>
+    <t>DASA-0004-2024</t>
+  </si>
+  <si>
+    <t>2024-01-04</t>
+  </si>
+  <si>
+    <t>COORDINACIÓN GENERAL ADMINISTRATIVA</t>
+  </si>
+  <si>
+    <t>DASA-0077-2023</t>
+  </si>
+  <si>
+    <t>2023-05-27</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN DE DEUDA PÚBLICA</t>
+  </si>
+  <si>
+    <t>DASA-0078-2023</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN DE PRESUPUESTO Y CONTROL PRESUPUESTAL</t>
+  </si>
+  <si>
+    <t>DASA-0079-2023</t>
+  </si>
+  <si>
+    <t>PROCURADURÍA FISCAL</t>
+  </si>
+  <si>
+    <t>DASA-0080-2023</t>
+  </si>
+  <si>
+    <t>2023-05-29</t>
+  </si>
+  <si>
+    <t>DASA-0081-2023</t>
   </si>
   <si>
     <t>DIRECCIÓN DE ADMINISTRACIÓN FINANCIERA</t>
   </si>
   <si>
-    <t>DCCP-0269-2023</t>
-  </si>
-  <si>
-    <t>2023-03-23</t>
-  </si>
-  <si>
-    <t>PROCURADURÍA FISCAL</t>
-  </si>
-  <si>
-    <t>DCCP-0270-2023</t>
-  </si>
-  <si>
-    <t>2023-03-22</t>
-  </si>
-  <si>
-    <t>DAF-659-2023</t>
-  </si>
-  <si>
-    <t>2023-03-28</t>
+    <t>DASA-0082-2023</t>
+  </si>
+  <si>
+    <t>DASA-0100-2023</t>
+  </si>
+  <si>
+    <t>2023-05-31</t>
+  </si>
+  <si>
+    <t>DASA-0130-2023</t>
+  </si>
+  <si>
+    <t>2023-06-07</t>
+  </si>
+  <si>
+    <t>DASA-0242-2023</t>
+  </si>
+  <si>
+    <t>2023-06-30</t>
+  </si>
+  <si>
+    <t>DASA-0248-2023</t>
+  </si>
+  <si>
+    <t>2023-07-04</t>
+  </si>
+  <si>
+    <t>DASA-0249-2023</t>
+  </si>
+  <si>
+    <t>DASA-0250-2023</t>
+  </si>
+  <si>
+    <t>DASA-0254-2023</t>
+  </si>
+  <si>
+    <t>DASA-0255-2023</t>
+  </si>
+  <si>
+    <t>2023-07-07</t>
+  </si>
+  <si>
+    <t>DASA-0269-2023</t>
+  </si>
+  <si>
+    <t>2023-07-10</t>
+  </si>
+  <si>
+    <t>DASA-0272-2023</t>
+  </si>
+  <si>
+    <t>DASA-0280-2023</t>
+  </si>
+  <si>
+    <t>2023-07-13</t>
+  </si>
+  <si>
+    <t>CGA-0228-2023</t>
+  </si>
+  <si>
+    <t>DAF-1067-2023</t>
+  </si>
+  <si>
+    <t>2023-06-01</t>
+  </si>
+  <si>
+    <t>DCCP-0480-2023</t>
+  </si>
+  <si>
+    <t>DDPYPF-090-2023</t>
+  </si>
+  <si>
+    <t>2023-06-05</t>
+  </si>
+  <si>
+    <t>DDPYPF-092-2023</t>
+  </si>
+  <si>
+    <t>2023-06-19</t>
+  </si>
+  <si>
+    <t>DPCP-348-2023</t>
+  </si>
+  <si>
+    <t>Auditoría Superior de la Federación ASF</t>
+  </si>
+  <si>
+    <t>,kj</t>
+  </si>
+  <si>
+    <t>Entrega 1</t>
+  </si>
+  <si>
+    <t>Secretaría de la Función Pública SFP</t>
+  </si>
+  <si>
+    <t>jfvgnkdfvk</t>
   </si>
   <si>
     <t>Contraloría y Transparencia Gubernamental Gobierno del Estado de Nuevo León CTG</t>
   </si>
   <si>
-    <t>DCCP-0312-2023</t>
-  </si>
-  <si>
-    <t>397/2023</t>
-  </si>
-  <si>
-    <t>2023-03-29</t>
-  </si>
-  <si>
-    <t>Recomendación</t>
-  </si>
-  <si>
-    <t>En seguimiento</t>
-  </si>
-  <si>
-    <t>2022-A-19000-19-1342-01-001</t>
-  </si>
-  <si>
-    <t>Para que el Gobierno del Estado de Nuevo León instrumente mecanismos de control y seguimiento que permitan conciliar, actualizar y validar el importe reportado a la Secretaría de Educación Pública de las transferencias de recursos estatales convenidos de los Subsidios Federales para Organismos Descentralizados Estatales, con el propósito de contribuir de manera proactiva al cumplimiento de los objetivos del programa y del marco normativo que lo rige.Los términos de esta recomendación y los mecanismos para su atención, por parte de la entidad fiscalizada, quedan asentados en el Acta de la Reunión de Presentación de Resultados Finales y Observaciones Preliminares en los términos del artículo 42 de la Ley de Fiscalización y Rendición de Cuentas de la Federación.</t>
-  </si>
-  <si>
-    <t>N/A</t>
+    <t>DASA-0122-2023</t>
+  </si>
+  <si>
+    <t>65/2023</t>
+  </si>
+  <si>
+    <t>2023-06-08</t>
+  </si>
+  <si>
+    <t>2023-06-09</t>
+  </si>
+  <si>
+    <t>Auditoria Superior del Estado de Nuevo Leon ASENL</t>
+  </si>
+  <si>
+    <t>2024-04-13</t>
+  </si>
+  <si>
+    <t>2024-04-11</t>
+  </si>
+  <si>
+    <t>2024-04-08</t>
+  </si>
+  <si>
+    <t>Solicitud de información' relativa a la Auditoría 1326, Cumplimiento de las Disposiciones Establecidas en la Ley de Disciplina Financiera de las Entidades Federativas y los Municipios</t>
+  </si>
+  <si>
+    <t>Solicitud de información relativa a la Auditoría 1326, Cumplimiento de las Disposiciones Establecidas en · la Ley de Disciplina Financiera de las Entidades Federativas y los Municipios</t>
+  </si>
+  <si>
+    <t>Solicitud de información relativa a la Auditoría 1326, Cumplimiento de las Disposiciones Establecidas en la Ley de Disciplina Financiera de las Entidades Federativas y los Municipios</t>
+  </si>
+  <si>
+    <t>Solicitud de información relativa a la Auditoría 1326, Cumplimiento de las Disposiciones Establecidas en la Ley de Disciplina Financiera de las 'Entidades Federativas y los Municipios</t>
+  </si>
+  <si>
+    <t>En alcance al oficio DASA-0081/2023, relativa a la Auditoría 1326, Cumplimiento de las Disposiciones Establecidas en la Ley de Disciplina Financiera de las Entidades Federativas y los Municipios</t>
+  </si>
+  <si>
+    <t>Solicitud de información relativa a la1 Auditoría 1326, Cumplimiento de las Disposiciones Establecidas en la Ley de Disciplina Financiera de las Entidades Federativas y los Municipios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solicitud de información complementaria a la 
+Auditoría 1326, cumplimiento de las Disposiciones Establecidas en al Ley de Disciplina Financiera de las Entidades Federativas y los Municipios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solicitud de información complementaria a la 
+Auditoría 1326, cumplimiento de las Disposiciones Establecidas en al Ley de Disciplina Financiera de las Entidades Federativas y los Municipios 
+</t>
+  </si>
+  <si>
+    <t>Se otorga prórroga</t>
   </si>
 </sst>
 </file>
@@ -295,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -310,8 +486,8 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -321,9 +497,6 @@
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,10 +831,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AM12"/>
+  <dimension ref="A1:AU28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="AE1">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.7265625" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -669,40 +842,47 @@
     <col min="1" max="1" width="19.1796875" customWidth="true" style="0"/>
     <col min="2" max="2" width="22.1796875" customWidth="true" style="0"/>
     <col min="3" max="3" width="22.1796875" customWidth="true" style="0"/>
-    <col min="5" max="5" width="28.90625" customWidth="true" style="0"/>
-    <col min="6" max="6" width="15" customWidth="true" style="0"/>
-    <col min="7" max="7" width="12.54296875" customWidth="true" style="0"/>
-    <col min="8" max="8" width="14.7265625" customWidth="true" style="0"/>
-    <col min="9" max="9" width="18.81640625" customWidth="true" style="0"/>
-    <col min="10" max="10" width="10.36328125" customWidth="true" style="0"/>
-    <col min="12" max="12" width="28.36328125" customWidth="true" style="0"/>
-    <col min="13" max="13" width="20.1796875" customWidth="true" style="0"/>
-    <col min="14" max="14" width="16.1796875" customWidth="true" style="0"/>
-    <col min="15" max="15" width="19.36328125" customWidth="true" style="0"/>
-    <col min="16" max="16" width="20.90625" customWidth="true" style="0"/>
-    <col min="17" max="17" width="20.90625" customWidth="true" style="0"/>
-    <col min="19" max="19" width="22" customWidth="true" style="0"/>
-    <col min="20" max="20" width="13.90625" customWidth="true" style="0"/>
+    <col min="4" max="4" width="22.1796875" customWidth="true" style="0"/>
+    <col min="5" max="5" width="22.1796875" customWidth="true" style="0"/>
+    <col min="6" max="6" width="22.1796875" customWidth="true" style="0"/>
+    <col min="8" max="8" width="28.90625" customWidth="true" style="0"/>
+    <col min="9" max="9" width="15" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12.54296875" customWidth="true" style="0"/>
+    <col min="11" max="11" width="14.7265625" customWidth="true" style="0"/>
+    <col min="13" max="13" width="28.36328125" customWidth="true" style="0"/>
+    <col min="14" max="14" width="20.1796875" customWidth="true" style="0"/>
+    <col min="15" max="15" width="16.1796875" customWidth="true" style="0"/>
+    <col min="16" max="16" width="19.36328125" customWidth="true" style="0"/>
+    <col min="18" max="18" width="22" customWidth="true" style="0"/>
+    <col min="19" max="19" width="13.90625" customWidth="true" style="0"/>
+    <col min="20" max="20" width="11.453125" customWidth="true" style="0"/>
     <col min="21" max="21" width="11.453125" customWidth="true" style="0"/>
     <col min="22" max="22" width="12.54296875" customWidth="true" style="0"/>
     <col min="23" max="23" width="14.7265625" customWidth="true" style="0"/>
     <col min="24" max="24" width="18.26953125" customWidth="true" style="0"/>
-    <col min="26" max="26" width="18" customWidth="true" style="0"/>
-    <col min="27" max="27" width="25.81640625" customWidth="true" style="0"/>
-    <col min="28" max="28" width="7.54296875" customWidth="true" style="0"/>
-    <col min="29" max="29" width="21.1796875" customWidth="true" style="0"/>
-    <col min="30" max="30" width="32.81640625" customWidth="true" style="0"/>
-    <col min="31" max="31" width="24.453125" customWidth="true" style="0"/>
+    <col min="26" max="26" width="19" customWidth="true" style="0"/>
+    <col min="27" max="27" width="19" customWidth="true" style="0"/>
+    <col min="28" max="28" width="19" customWidth="true" style="0"/>
+    <col min="29" max="29" width="19" customWidth="true" style="0"/>
+    <col min="30" max="30" width="19" customWidth="true" style="0"/>
+    <col min="31" max="31" width="19" customWidth="true" style="0"/>
     <col min="32" max="32" width="19" customWidth="true" style="0"/>
-    <col min="34" max="34" width="27.54296875" customWidth="true" style="0"/>
-    <col min="35" max="35" width="15" customWidth="true" style="0"/>
-    <col min="36" max="36" width="12.1796875" customWidth="true" style="0"/>
-    <col min="37" max="37" width="18.81640625" customWidth="true" style="0"/>
-    <col min="38" max="38" width="15.08984375" customWidth="true" style="0"/>
-    <col min="39" max="39" width="14.7265625" customWidth="true" style="0"/>
+    <col min="34" max="34" width="18" customWidth="true" style="0"/>
+    <col min="35" max="35" width="25.81640625" customWidth="true" style="0"/>
+    <col min="36" max="36" width="7.54296875" customWidth="true" style="0"/>
+    <col min="37" max="37" width="21.1796875" customWidth="true" style="0"/>
+    <col min="38" max="38" width="32.81640625" customWidth="true" style="0"/>
+    <col min="39" max="39" width="24.453125" customWidth="true" style="0"/>
+    <col min="40" max="40" width="19" customWidth="true" style="0"/>
+    <col min="42" max="42" width="27.54296875" customWidth="true" style="0"/>
+    <col min="43" max="43" width="15" customWidth="true" style="0"/>
+    <col min="44" max="44" width="12.1796875" customWidth="true" style="0"/>
+    <col min="45" max="45" width="18.81640625" customWidth="true" style="0"/>
+    <col min="46" max="46" width="15.08984375" customWidth="true" style="0"/>
+    <col min="47" max="47" width="14.7265625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:47">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,338 +890,919 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:47">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="H9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="L9" s="9" t="s">
+      <c r="K9" s="8"/>
+      <c r="M9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="S9" s="9" t="s">
+      <c r="R9" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="S9" s="9"/>
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
-      <c r="Z9" s="8" t="s">
+      <c r="Z9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AH9" s="7" t="s">
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AH9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="AI9" s="7"/>
-      <c r="AJ9" s="7"/>
-      <c r="AK9" s="7"/>
-      <c r="AL9" s="7"/>
-      <c r="AM9" s="7"/>
-    </row>
-    <row r="10" spans="1:39">
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8"/>
+      <c r="AP9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="7"/>
+      <c r="AS9" s="7"/>
+      <c r="AT9" s="7"/>
+      <c r="AU9" s="7"/>
+    </row>
+    <row r="10" spans="1:47" customHeight="1" ht="15.5">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="H10" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="U10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="X10" s="2" t="s">
+      <c r="AC10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC10" s="2" t="s">
+      <c r="AF10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AD10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF10" s="2" t="s">
+      <c r="AH10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AH10" s="2" t="s">
+      <c r="AI10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AI10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM10" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39">
+      <c r="AQ10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11"/>
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
       <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="s">
-        <v>40</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F11"/>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="K11" t="s">
+        <v>50</v>
       </c>
       <c r="M11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="N11" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" t="s">
+        <v>65</v>
+      </c>
+      <c r="R11" t="s">
+        <v>91</v>
+      </c>
+      <c r="S11" t="s">
+        <v>92</v>
+      </c>
+      <c r="T11"/>
+      <c r="U11" t="s">
+        <v>93</v>
+      </c>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Z11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB11">
+        <v>123</v>
+      </c>
+      <c r="AC11">
+        <v>123</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS11"/>
+      <c r="AT11"/>
+      <c r="AU11"/>
+    </row>
+    <row r="12" spans="1:47">
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12"/>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N12" t="s">
+        <v>83</v>
+      </c>
+      <c r="O12" t="s">
+        <v>84</v>
+      </c>
+      <c r="P12" t="s">
+        <v>84</v>
+      </c>
+      <c r="R12" t="s">
+        <v>94</v>
+      </c>
+      <c r="S12" t="s">
+        <v>95</v>
+      </c>
+      <c r="T12"/>
+      <c r="U12" t="s">
+        <v>93</v>
+      </c>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="AP12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>105</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47">
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" t="s">
         <v>45</v>
       </c>
-      <c r="O11" t="s">
+      <c r="K13" t="s">
         <v>45</v>
       </c>
-      <c r="P11" t="s">
+      <c r="M13" t="s">
+        <v>48</v>
+      </c>
+      <c r="N13" t="s">
+        <v>85</v>
+      </c>
+      <c r="O13" t="s">
+        <v>84</v>
+      </c>
+      <c r="P13" t="s">
+        <v>84</v>
+      </c>
+      <c r="R13" t="s">
+        <v>96</v>
+      </c>
+      <c r="S13" t="s">
+        <v>97</v>
+      </c>
+      <c r="T13" t="s">
+        <v>98</v>
+      </c>
+      <c r="U13" t="s">
+        <v>93</v>
+      </c>
+      <c r="V13" t="s">
+        <v>99</v>
+      </c>
+      <c r="W13" t="s">
+        <v>100</v>
+      </c>
+      <c r="X13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR13" t="s">
         <v>45</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="AS13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47">
+      <c r="H14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" t="s">
         <v>45</v>
       </c>
-      <c r="S11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T11" t="s">
-        <v>47</v>
-      </c>
-      <c r="U11" t="s">
+      <c r="K14" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O14" t="s">
+        <v>87</v>
+      </c>
+      <c r="P14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47">
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" t="s">
+        <v>54</v>
+      </c>
+      <c r="N15" t="s">
+        <v>88</v>
+      </c>
+      <c r="O15" t="s">
+        <v>89</v>
+      </c>
+      <c r="P15" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>108</v>
+      </c>
+      <c r="AT15"/>
+      <c r="AU15"/>
+    </row>
+    <row r="16" spans="1:47">
+      <c r="H16" t="s">
         <v>48</v>
       </c>
-      <c r="V11" t="s">
-        <v>49</v>
-      </c>
-      <c r="W11" t="s">
-        <v>49</v>
-      </c>
-      <c r="X11" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB11">
-        <v>0.0</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD11" t="s">
+      <c r="I16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" t="s">
+        <v>90</v>
+      </c>
+      <c r="O16" t="s">
+        <v>84</v>
+      </c>
+      <c r="P16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT16"/>
+      <c r="AU16"/>
+    </row>
+    <row r="17" spans="1:47">
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" t="s">
         <v>53</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="K17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:47">
+      <c r="H18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:47">
+      <c r="H19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AT19"/>
+      <c r="AU19"/>
+    </row>
+    <row r="20" spans="1:47">
+      <c r="H20" t="s">
         <v>54</v>
       </c>
-      <c r="AF11">
-        <v>1</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AK11"/>
-      <c r="AL11" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39">
-      <c r="E12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK12"/>
-      <c r="AL12"/>
-      <c r="AM12"/>
+      <c r="I20" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>111</v>
+      </c>
+      <c r="AT20"/>
+      <c r="AU20"/>
+    </row>
+    <row r="21" spans="1:47">
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS21" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT21"/>
+      <c r="AU21"/>
+    </row>
+    <row r="22" spans="1:47">
+      <c r="H22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" t="s">
+        <v>71</v>
+      </c>
+      <c r="K22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT22"/>
+      <c r="AU22"/>
+    </row>
+    <row r="23" spans="1:47">
+      <c r="H23" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS23" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT23"/>
+      <c r="AU23"/>
+    </row>
+    <row r="24" spans="1:47">
+      <c r="H24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS24" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT24"/>
+      <c r="AU24"/>
+    </row>
+    <row r="25" spans="1:47">
+      <c r="H25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" t="s">
+        <v>76</v>
+      </c>
+      <c r="K25" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP25" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR25" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS25" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT25"/>
+      <c r="AU25"/>
+    </row>
+    <row r="26" spans="1:47">
+      <c r="H26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" t="s">
+        <v>77</v>
+      </c>
+      <c r="J26" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ26" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR26" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS26" t="s">
+        <v>111</v>
+      </c>
+      <c r="AT26"/>
+      <c r="AU26"/>
+    </row>
+    <row r="27" spans="1:47">
+      <c r="H27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" t="s">
+        <v>78</v>
+      </c>
+      <c r="K27" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR27" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS27" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT27"/>
+      <c r="AU27"/>
+    </row>
+    <row r="28" spans="1:47">
+      <c r="H28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" t="s">
+        <v>80</v>
+      </c>
+      <c r="J28" t="s">
+        <v>81</v>
+      </c>
+      <c r="K28" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ28" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR28" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS28" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT28"/>
+      <c r="AU28"/>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="AH9:AM9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="S9:X9"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="AP9:AU9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="R9:X9"/>
+    <mergeCell ref="AH9:AN9"/>
+    <mergeCell ref="M9:P9"/>
     <mergeCell ref="Z9:AF9"/>
-    <mergeCell ref="L9:Q9"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>